<commit_message>
added rapor-tarihi special field control, improved handling of comboboxes with 1 value by making selecting it automatically, other minor changes
</commit_message>
<xml_diff>
--- a/implicaspection/report-exports/a2yorumkod-Bericht2_MitKommentaren220200601-22:25:22.xlsx
+++ b/implicaspection/report-exports/a2yorumkod-Bericht2_MitKommentaren220200601-22:25:22.xlsx
@@ -112,6 +112,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">???combo???Müşteri Adı???musteri-adi</t>
         </r>
@@ -1319,10 +1320,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="127">
-  <si>
-    <t xml:space="preserve">şablondur</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="113">
   <si>
     <t xml:space="preserve"> GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ</t>
   </si>
@@ -1424,6 +1422,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -1447,7 +1448,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">KAYNAKÇI TESTİ</t>
+    <t xml:space="preserve">DENEME PROJESİ</t>
   </si>
   <si>
     <r>
@@ -1473,6 +1474,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">100%</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -1635,7 +1639,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">After Welding</t>
+    <t xml:space="preserve">Deneme</t>
   </si>
   <si>
     <r>
@@ -1708,9 +1712,6 @@
       </rPr>
       <t xml:space="preserve">Stage Of Examination</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Untreated</t>
   </si>
   <si>
     <r>
@@ -1860,14 +1861,8 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">NAWOO Sn:1701020</t>
-  </si>
-  <si>
     <t xml:space="preserve">Akım Tipi
 Current Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC</t>
   </si>
   <si>
     <r>
@@ -2847,42 +2842,6 @@
   </si>
   <si>
     <t xml:space="preserve">Doküman No: F.02 Yayın Tarihi : 01.05.2018 Revizyon No :01 Revizyon Tarihi :19.03.2019</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>P-101-004</t>
-  </si>
-  <si>
-    <t>Deneme</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>KAYNAK+HAZ</t>
-  </si>
-  <si>
-    <t>DENEME PROJESİ</t>
-  </si>
-  <si>
-    <t>1200 Lux</t>
-  </si>
-  <si>
-    <t>TS EN ISO 23278 Class B</t>
-  </si>
-  <si>
-    <t>100%</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>TS EN ISO 17638</t>
-  </si>
-  <si>
-    <t>TAG GEMİ</t>
   </si>
 </sst>
 </file>
@@ -2895,7 +2854,7 @@
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2997,6 +2956,13 @@
       <charset val="162"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFCE181E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="8"/>
       <name val="Arial"/>
@@ -3053,6 +3019,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -3062,7 +3029,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3072,7 +3039,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD1CD"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFFCD4D1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD4D1"/>
+        <bgColor rgb="FFFFD1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF21409A"/>
+        <bgColor rgb="FF003366"/>
       </patternFill>
     </fill>
   </fills>
@@ -3236,7 +3221,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3397,6 +3382,18 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3425,7 +3422,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3453,7 +3450,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3465,7 +3462,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3473,7 +3470,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3485,7 +3482,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3553,7 +3550,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -3571,7 +3568,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFFCD4D1"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -3600,9 +3597,9 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF21409A"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -3620,9 +3617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>13680</xdr:colOff>
+      <xdr:colOff>13320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>197640</xdr:rowOff>
+      <xdr:rowOff>197280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3636,7 +3633,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2276280" y="5213880"/>
-          <a:ext cx="1520640" cy="1078920"/>
+          <a:ext cx="1520280" cy="1078560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3657,9 +3654,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>149760</xdr:colOff>
+      <xdr:colOff>149400</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3673,7 +3670,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="74160" y="5230080"/>
-          <a:ext cx="1781640" cy="901080"/>
+          <a:ext cx="1781280" cy="900720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3693,48 +3690,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO429"/>
+  <dimension ref="A1:AO74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="AE20" activeCellId="0" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="7.27" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="3" customWidth="true" hidden="false" style="1" width="5.28" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="0.82" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="4.71" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="0.82" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="4.17" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="3.27" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="5.55" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="3.45" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="1" width="5.72" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="4.82" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="15" customWidth="true" hidden="false" style="1" width="0.82" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="8.72" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="3.71" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="10.73" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="4.82" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="3.83" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="1" width="3.45" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="1" width="0.82" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="10.73" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="24" customWidth="true" hidden="false" style="1" width="2.46" collapsed="true" outlineLevel="0"/>
-    <col min="25" max="25" customWidth="true" hidden="false" style="1" width="5.72" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="4.71" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="6.72" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="7.82" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="34" customWidth="true" hidden="false" style="1" width="8.82" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="16.81" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="1025" customWidth="true" hidden="false" style="1" width="8.82" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="0.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="0.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="3.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="3.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="4.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="1" width="0.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="4.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="3.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="0.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="2.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="5.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="29" style="1" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="36" style="1" width="8.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -3742,7 +3737,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -3774,7 +3769,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -3799,12 +3794,12 @@
     </row>
     <row r="3" s="10" customFormat="true" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>126</v>
+        <v>3</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -3819,23 +3814,23 @@
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="8" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="9" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="AB3" s="9"/>
     </row>
@@ -3846,7 +3841,7 @@
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -3866,13 +3861,13 @@
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
       <c r="T4" s="14" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="U4" s="14"/>
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
       <c r="X4" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
@@ -3881,25 +3876,25 @@
       </c>
       <c r="AB4" s="15"/>
       <c r="AF4" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AG4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="AH4" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AI4" s="10" t="n">
         <v>2</v>
       </c>
       <c r="AJ4" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AK4" s="10" t="n">
         <v>3</v>
       </c>
       <c r="AN4" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AO4" s="10" t="n">
         <v>4</v>
@@ -3907,12 +3902,12 @@
     </row>
     <row r="5" s="10" customFormat="true" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -3927,18 +3922,18 @@
       <c r="O5" s="16"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
       <c r="T5" s="17" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="U5" s="17"/>
       <c r="V5" s="17"/>
       <c r="W5" s="17"/>
       <c r="X5" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
@@ -3947,26 +3942,26 @@
       </c>
       <c r="AB5" s="18"/>
       <c r="AG5" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AI5" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AK5" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AO5" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" s="10" customFormat="true" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="12" t="s">
-        <v>125</v>
+        <v>24</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -3981,18 +3976,18 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
       <c r="T6" s="17" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="U6" s="17"/>
       <c r="V6" s="17"/>
       <c r="W6" s="17"/>
       <c r="X6" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
@@ -4003,12 +3998,12 @@
     </row>
     <row r="7" s="10" customFormat="true" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="20" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -4023,12 +4018,12 @@
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
       <c r="T7" s="22" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="U7" s="22"/>
       <c r="V7" s="22"/>
@@ -4099,7 +4094,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="25" t="s">
-        <v>119</v>
+        <v>37</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
@@ -4128,7 +4123,7 @@
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="25" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
@@ -4136,7 +4131,7 @@
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
@@ -4144,7 +4139,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="25" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
@@ -4152,28 +4147,28 @@
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
       <c r="W10" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="X10" s="27"/>
       <c r="Y10" s="27"/>
       <c r="Z10" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AA10" s="26"/>
       <c r="AB10" s="26"/>
       <c r="AF10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
@@ -4181,7 +4176,7 @@
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
       <c r="K11" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
@@ -4189,7 +4184,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="25" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
@@ -4205,7 +4200,7 @@
     </row>
     <row r="12" s="30" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -4217,41 +4212,39 @@
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
       <c r="K12" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
-      <c r="Q12" s="28" t="s">
-        <v>118</v>
-      </c>
+      <c r="Q12" s="28"/>
       <c r="R12" s="28"/>
       <c r="S12" s="28"/>
       <c r="T12" s="28"/>
       <c r="U12" s="28"/>
       <c r="V12" s="28"/>
       <c r="W12" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA12" s="29"/>
       <c r="AB12" s="29"/>
     </row>
     <row r="13" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
@@ -4259,7 +4252,7 @@
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
       <c r="K13" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
@@ -4273,25 +4266,25 @@
       <c r="U13" s="25"/>
       <c r="V13" s="25"/>
       <c r="W13" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X13" s="27"/>
       <c r="Y13" s="27"/>
       <c r="Z13" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AA13" s="26"/>
       <c r="AB13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" s="31"/>
       <c r="G14" s="31"/>
@@ -4299,7 +4292,7 @@
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
       <c r="K14" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
@@ -4313,17 +4306,17 @@
       <c r="U14" s="32"/>
       <c r="V14" s="32"/>
       <c r="W14" s="33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="X14" s="33"/>
       <c r="Y14" s="33"/>
       <c r="Z14" s="34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AA14" s="34"/>
       <c r="AB14" s="34"/>
       <c r="AF14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4335,7 +4328,7 @@
       <c r="F15" s="35"/>
       <c r="G15" s="35"/>
       <c r="H15" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I15" s="36"/>
       <c r="J15" s="36"/>
@@ -4346,7 +4339,7 @@
       <c r="O15" s="36"/>
       <c r="P15" s="36"/>
       <c r="Q15" s="37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R15" s="37"/>
       <c r="S15" s="37"/>
@@ -4378,11 +4371,11 @@
       <c r="O16" s="36"/>
       <c r="P16" s="36"/>
       <c r="Q16" s="38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R16" s="38"/>
       <c r="S16" s="39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="T16" s="39"/>
       <c r="U16" s="39"/>
@@ -4393,6 +4386,9 @@
       <c r="Z16" s="39"/>
       <c r="AA16" s="39"/>
       <c r="AB16" s="39"/>
+      <c r="AE16" s="40"/>
+      <c r="AF16" s="41"/>
+      <c r="AG16" s="42"/>
     </row>
     <row r="17" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="35"/>
@@ -4411,22 +4407,22 @@
       <c r="N17" s="36"/>
       <c r="O17" s="36"/>
       <c r="P17" s="36"/>
-      <c r="Q17" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="R17" s="40"/>
-      <c r="S17" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="T17" s="41"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="41"/>
-      <c r="Y17" s="41"/>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="41"/>
-      <c r="AB17" s="41"/>
+      <c r="Q17" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="R17" s="43"/>
+      <c r="S17" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="T17" s="44"/>
+      <c r="U17" s="44"/>
+      <c r="V17" s="44"/>
+      <c r="W17" s="44"/>
+      <c r="X17" s="44"/>
+      <c r="Y17" s="44"/>
+      <c r="Z17" s="44"/>
+      <c r="AA17" s="44"/>
+      <c r="AB17" s="44"/>
     </row>
     <row r="18" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="35"/>
@@ -4445,12 +4441,12 @@
       <c r="N18" s="36"/>
       <c r="O18" s="36"/>
       <c r="P18" s="36"/>
-      <c r="Q18" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="R18" s="40"/>
+      <c r="Q18" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="R18" s="43"/>
       <c r="S18" s="39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T18" s="39"/>
       <c r="U18" s="39"/>
@@ -4479,161 +4475,161 @@
       <c r="N19" s="36"/>
       <c r="O19" s="36"/>
       <c r="P19" s="36"/>
-      <c r="Q19" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="R19" s="42"/>
-      <c r="S19" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="T19" s="43"/>
-      <c r="U19" s="43"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="43"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="43"/>
-      <c r="Z19" s="43"/>
-      <c r="AA19" s="43"/>
-      <c r="AB19" s="43"/>
+      <c r="Q19" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="R19" s="45"/>
+      <c r="S19" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="T19" s="46"/>
+      <c r="U19" s="46"/>
+      <c r="V19" s="46"/>
+      <c r="W19" s="46"/>
+      <c r="X19" s="46"/>
+      <c r="Y19" s="46"/>
+      <c r="Z19" s="46"/>
+      <c r="AA19" s="46"/>
+      <c r="AB19" s="46"/>
     </row>
     <row r="20" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-      <c r="U20" s="45"/>
-      <c r="V20" s="45"/>
-      <c r="W20" s="45"/>
-      <c r="X20" s="45"/>
-      <c r="Y20" s="45"/>
-      <c r="Z20" s="45"/>
-      <c r="AA20" s="45"/>
-      <c r="AB20" s="45"/>
+      <c r="A20" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
     </row>
     <row r="21" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="47" t="n">
+      <c r="A21" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="50" t="n">
         <v>43754</v>
       </c>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="47"/>
-      <c r="V21" s="47"/>
-      <c r="W21" s="47"/>
-      <c r="X21" s="47"/>
-      <c r="Y21" s="47"/>
-      <c r="Z21" s="47"/>
-      <c r="AA21" s="47"/>
-      <c r="AB21" s="47"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="50"/>
+      <c r="Z21" s="50"/>
+      <c r="AA21" s="50"/>
+      <c r="AB21" s="50"/>
     </row>
     <row r="22" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
-      <c r="Q22" s="49"/>
-      <c r="R22" s="49"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="49"/>
-      <c r="U22" s="49"/>
-      <c r="V22" s="49"/>
-      <c r="W22" s="49"/>
-      <c r="X22" s="49"/>
-      <c r="Y22" s="49"/>
-      <c r="Z22" s="49"/>
-      <c r="AA22" s="49"/>
-      <c r="AB22" s="49"/>
+      <c r="A22" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="52"/>
+      <c r="S22" s="52"/>
+      <c r="T22" s="52"/>
+      <c r="U22" s="52"/>
+      <c r="V22" s="52"/>
+      <c r="W22" s="52"/>
+      <c r="X22" s="52"/>
+      <c r="Y22" s="52"/>
+      <c r="Z22" s="52"/>
+      <c r="AA22" s="52"/>
+      <c r="AB22" s="52"/>
     </row>
     <row r="23" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="50"/>
-      <c r="S23" s="50"/>
-      <c r="T23" s="50"/>
-      <c r="U23" s="50"/>
-      <c r="V23" s="50"/>
-      <c r="W23" s="50"/>
-      <c r="X23" s="50"/>
-      <c r="Y23" s="50"/>
-      <c r="Z23" s="50"/>
-      <c r="AA23" s="50"/>
-      <c r="AB23" s="50"/>
+      <c r="A23" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53"/>
+      <c r="T23" s="53"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
+      <c r="Y23" s="53"/>
+      <c r="Z23" s="53"/>
+      <c r="AA23" s="53"/>
+      <c r="AB23" s="53"/>
     </row>
     <row r="24" s="10" customFormat="true" ht="28.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="51" t="s">
-        <v>82</v>
+      <c r="A24" s="54" t="s">
+        <v>80</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
@@ -4642,12 +4638,12 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
       <c r="I24" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J24" s="27"/>
       <c r="K24" s="27"/>
       <c r="L24" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
@@ -4655,776 +4651,776 @@
       <c r="P24" s="27"/>
       <c r="Q24" s="27"/>
       <c r="R24" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="S24" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T24" s="27"/>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
       <c r="W24" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X24" s="27"/>
       <c r="Y24" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Z24" s="27"/>
       <c r="AA24" s="27"/>
-      <c r="AB24" s="52" t="s">
-        <v>90</v>
+      <c r="AB24" s="55" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="53" t="n">
+      <c r="A25" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="58" t="n">
+        <v>300</v>
+      </c>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58" t="n">
+        <v>12</v>
+      </c>
+      <c r="S25" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="58"/>
+      <c r="X25" s="58"/>
+      <c r="Y25" s="58"/>
+      <c r="Z25" s="58"/>
+      <c r="AA25" s="58"/>
+      <c r="AB25" s="60" t="s">
         <v>91</v>
-      </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="55" t="n">
-        <v>300</v>
-      </c>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="55" t="n">
-        <v>12</v>
-      </c>
-      <c r="S25" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="T25" s="56"/>
-      <c r="U25" s="56"/>
-      <c r="V25" s="56"/>
-      <c r="W25" s="55"/>
-      <c r="X25" s="55"/>
-      <c r="Y25" s="55"/>
-      <c r="Z25" s="55"/>
-      <c r="AA25" s="55"/>
-      <c r="AB25" s="57" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="53" t="n">
+      <c r="A26" s="56" t="n">
         <v>2</v>
       </c>
-      <c r="B26" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="55" t="n">
+      <c r="B26" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="58" t="n">
         <v>300</v>
       </c>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="55" t="n">
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="58" t="n">
         <v>12</v>
       </c>
-      <c r="S26" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="T26" s="56"/>
-      <c r="U26" s="56"/>
-      <c r="V26" s="56"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="55"/>
-      <c r="Y26" s="55"/>
-      <c r="Z26" s="55"/>
-      <c r="AA26" s="55"/>
-      <c r="AB26" s="57" t="s">
-        <v>93</v>
+      <c r="S26" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="T26" s="59"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="58"/>
+      <c r="X26" s="58"/>
+      <c r="Y26" s="58"/>
+      <c r="Z26" s="58"/>
+      <c r="AA26" s="58"/>
+      <c r="AB26" s="60" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="53" t="n">
+      <c r="A27" s="56" t="n">
         <v>3</v>
       </c>
-      <c r="B27" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="55" t="n">
+      <c r="B27" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="58" t="n">
         <v>300</v>
       </c>
-      <c r="J27" s="55"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="M27" s="55"/>
-      <c r="N27" s="55"/>
-      <c r="O27" s="55"/>
-      <c r="P27" s="55"/>
-      <c r="Q27" s="55"/>
-      <c r="R27" s="55" t="n">
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58" t="n">
         <v>12</v>
       </c>
-      <c r="S27" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="T27" s="56"/>
-      <c r="U27" s="56"/>
-      <c r="V27" s="56"/>
-      <c r="W27" s="55"/>
-      <c r="X27" s="55"/>
-      <c r="Y27" s="55"/>
-      <c r="Z27" s="55"/>
-      <c r="AA27" s="55"/>
-      <c r="AB27" s="57" t="s">
-        <v>93</v>
+      <c r="S27" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="T27" s="59"/>
+      <c r="U27" s="59"/>
+      <c r="V27" s="59"/>
+      <c r="W27" s="58"/>
+      <c r="X27" s="58"/>
+      <c r="Y27" s="58"/>
+      <c r="Z27" s="58"/>
+      <c r="AA27" s="58"/>
+      <c r="AB27" s="60" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="53" t="n">
+      <c r="A28" s="56" t="n">
         <v>4</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="58" t="n">
+        <v>300</v>
+      </c>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="58" t="n">
+        <v>12</v>
+      </c>
+      <c r="S28" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="T28" s="59"/>
+      <c r="U28" s="59"/>
+      <c r="V28" s="59"/>
+      <c r="W28" s="58"/>
+      <c r="X28" s="58"/>
+      <c r="Y28" s="58"/>
+      <c r="Z28" s="58"/>
+      <c r="AA28" s="58"/>
+      <c r="AB28" s="60" t="s">
         <v>91</v>
-      </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="55" t="n">
-        <v>300</v>
-      </c>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55" t="n">
-        <v>12</v>
-      </c>
-      <c r="S28" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="T28" s="56"/>
-      <c r="U28" s="56"/>
-      <c r="V28" s="56"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="55"/>
-      <c r="Y28" s="55"/>
-      <c r="Z28" s="55"/>
-      <c r="AA28" s="55"/>
-      <c r="AB28" s="57" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="53" t="n">
+      <c r="A29" s="56" t="n">
         <v>5</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="58" t="n">
+        <v>300</v>
+      </c>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="55" t="n">
-        <v>300</v>
-      </c>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
-      <c r="R29" s="55" t="n">
+      <c r="M29" s="58"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="58"/>
+      <c r="Q29" s="58"/>
+      <c r="R29" s="58" t="n">
         <v>12</v>
       </c>
-      <c r="S29" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="T29" s="56"/>
-      <c r="U29" s="56"/>
-      <c r="V29" s="56"/>
-      <c r="W29" s="55"/>
-      <c r="X29" s="55"/>
-      <c r="Y29" s="55"/>
-      <c r="Z29" s="55"/>
-      <c r="AA29" s="55"/>
-      <c r="AB29" s="57" t="s">
-        <v>93</v>
+      <c r="S29" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="T29" s="59"/>
+      <c r="U29" s="59"/>
+      <c r="V29" s="59"/>
+      <c r="W29" s="58"/>
+      <c r="X29" s="58"/>
+      <c r="Y29" s="58"/>
+      <c r="Z29" s="58"/>
+      <c r="AA29" s="58"/>
+      <c r="AB29" s="60" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="53" t="n">
+      <c r="A30" s="56" t="n">
         <v>6</v>
       </c>
-      <c r="B30" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="55" t="n">
+      <c r="B30" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="58" t="n">
         <v>300</v>
       </c>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="M30" s="55"/>
-      <c r="N30" s="55"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="55"/>
-      <c r="Q30" s="55"/>
-      <c r="R30" s="55" t="n">
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="58"/>
+      <c r="Q30" s="58"/>
+      <c r="R30" s="58" t="n">
         <v>12</v>
       </c>
-      <c r="S30" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="T30" s="56"/>
-      <c r="U30" s="56"/>
-      <c r="V30" s="56"/>
-      <c r="W30" s="55"/>
-      <c r="X30" s="55"/>
-      <c r="Y30" s="55"/>
-      <c r="Z30" s="55"/>
-      <c r="AA30" s="55"/>
-      <c r="AB30" s="57" t="s">
-        <v>93</v>
+      <c r="S30" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="T30" s="59"/>
+      <c r="U30" s="59"/>
+      <c r="V30" s="59"/>
+      <c r="W30" s="58"/>
+      <c r="X30" s="58"/>
+      <c r="Y30" s="58"/>
+      <c r="Z30" s="58"/>
+      <c r="AA30" s="58"/>
+      <c r="AB30" s="60" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="53" t="n">
+      <c r="A31" s="56" t="n">
         <v>7</v>
       </c>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="58" t="n">
+        <v>300</v>
+      </c>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="58"/>
+      <c r="R31" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="S31" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="55" t="n">
-        <v>300</v>
-      </c>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="M31" s="55"/>
-      <c r="N31" s="55"/>
-      <c r="O31" s="55"/>
-      <c r="P31" s="55"/>
-      <c r="Q31" s="55"/>
-      <c r="R31" s="55" t="n">
-        <v>4</v>
-      </c>
-      <c r="S31" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="T31" s="56"/>
-      <c r="U31" s="56"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="55"/>
-      <c r="X31" s="55"/>
-      <c r="Y31" s="55"/>
-      <c r="Z31" s="55"/>
-      <c r="AA31" s="55"/>
-      <c r="AB31" s="57" t="s">
-        <v>93</v>
+      <c r="T31" s="59"/>
+      <c r="U31" s="59"/>
+      <c r="V31" s="59"/>
+      <c r="W31" s="58"/>
+      <c r="X31" s="58"/>
+      <c r="Y31" s="58"/>
+      <c r="Z31" s="58"/>
+      <c r="AA31" s="58"/>
+      <c r="AB31" s="60" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="53" t="n">
+      <c r="A32" s="56" t="n">
         <v>8</v>
       </c>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="55"/>
-      <c r="M32" s="55"/>
-      <c r="N32" s="55"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="55"/>
-      <c r="Q32" s="55"/>
-      <c r="R32" s="55"/>
-      <c r="S32" s="56"/>
-      <c r="T32" s="56"/>
-      <c r="U32" s="56"/>
-      <c r="V32" s="56"/>
-      <c r="W32" s="55"/>
-      <c r="X32" s="55"/>
-      <c r="Y32" s="55"/>
-      <c r="Z32" s="55"/>
-      <c r="AA32" s="55"/>
-      <c r="AB32" s="57"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="58"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="58"/>
+      <c r="S32" s="59"/>
+      <c r="T32" s="59"/>
+      <c r="U32" s="59"/>
+      <c r="V32" s="59"/>
+      <c r="W32" s="58"/>
+      <c r="X32" s="58"/>
+      <c r="Y32" s="58"/>
+      <c r="Z32" s="58"/>
+      <c r="AA32" s="58"/>
+      <c r="AB32" s="60"/>
     </row>
     <row r="33" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="53" t="n">
+      <c r="A33" s="56" t="n">
         <v>9</v>
       </c>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="55"/>
-      <c r="N33" s="55"/>
-      <c r="O33" s="55"/>
-      <c r="P33" s="55"/>
-      <c r="Q33" s="55"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="56"/>
-      <c r="T33" s="56"/>
-      <c r="U33" s="56"/>
-      <c r="V33" s="56"/>
-      <c r="W33" s="55"/>
-      <c r="X33" s="55"/>
-      <c r="Y33" s="55"/>
-      <c r="Z33" s="55"/>
-      <c r="AA33" s="55"/>
-      <c r="AB33" s="57"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="58"/>
+      <c r="S33" s="59"/>
+      <c r="T33" s="59"/>
+      <c r="U33" s="59"/>
+      <c r="V33" s="59"/>
+      <c r="W33" s="58"/>
+      <c r="X33" s="58"/>
+      <c r="Y33" s="58"/>
+      <c r="Z33" s="58"/>
+      <c r="AA33" s="58"/>
+      <c r="AB33" s="60"/>
     </row>
     <row r="34" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="53" t="n">
+      <c r="A34" s="56" t="n">
         <v>10</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="55"/>
-      <c r="M34" s="55"/>
-      <c r="N34" s="55"/>
-      <c r="O34" s="55"/>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="55"/>
-      <c r="R34" s="55"/>
-      <c r="S34" s="56"/>
-      <c r="T34" s="56"/>
-      <c r="U34" s="56"/>
-      <c r="V34" s="56"/>
-      <c r="W34" s="55"/>
-      <c r="X34" s="55"/>
-      <c r="Y34" s="55"/>
-      <c r="Z34" s="55"/>
-      <c r="AA34" s="55"/>
-      <c r="AB34" s="57"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="59"/>
+      <c r="T34" s="59"/>
+      <c r="U34" s="59"/>
+      <c r="V34" s="59"/>
+      <c r="W34" s="58"/>
+      <c r="X34" s="58"/>
+      <c r="Y34" s="58"/>
+      <c r="Z34" s="58"/>
+      <c r="AA34" s="58"/>
+      <c r="AB34" s="60"/>
     </row>
     <row r="35" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="53" t="n">
+      <c r="A35" s="56" t="n">
         <v>11</v>
       </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="55"/>
-      <c r="M35" s="55"/>
-      <c r="N35" s="55"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="56"/>
-      <c r="T35" s="56"/>
-      <c r="U35" s="56"/>
-      <c r="V35" s="56"/>
-      <c r="W35" s="55"/>
-      <c r="X35" s="55"/>
-      <c r="Y35" s="55"/>
-      <c r="Z35" s="55"/>
-      <c r="AA35" s="55"/>
-      <c r="AB35" s="57"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="58"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="58"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="58"/>
+      <c r="Q35" s="58"/>
+      <c r="R35" s="58"/>
+      <c r="S35" s="59"/>
+      <c r="T35" s="59"/>
+      <c r="U35" s="59"/>
+      <c r="V35" s="59"/>
+      <c r="W35" s="58"/>
+      <c r="X35" s="58"/>
+      <c r="Y35" s="58"/>
+      <c r="Z35" s="58"/>
+      <c r="AA35" s="58"/>
+      <c r="AB35" s="60"/>
     </row>
     <row r="36" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="53" t="n">
+      <c r="A36" s="56" t="n">
         <v>12</v>
       </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="55"/>
-      <c r="S36" s="56"/>
-      <c r="T36" s="56"/>
-      <c r="U36" s="56"/>
-      <c r="V36" s="56"/>
-      <c r="W36" s="55"/>
-      <c r="X36" s="55"/>
-      <c r="Y36" s="55"/>
-      <c r="Z36" s="55"/>
-      <c r="AA36" s="55"/>
-      <c r="AB36" s="57"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="58"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="58"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="58"/>
+      <c r="R36" s="58"/>
+      <c r="S36" s="59"/>
+      <c r="T36" s="59"/>
+      <c r="U36" s="59"/>
+      <c r="V36" s="59"/>
+      <c r="W36" s="58"/>
+      <c r="X36" s="58"/>
+      <c r="Y36" s="58"/>
+      <c r="Z36" s="58"/>
+      <c r="AA36" s="58"/>
+      <c r="AB36" s="60"/>
     </row>
     <row r="37" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="53" t="n">
+      <c r="A37" s="56" t="n">
         <v>13</v>
       </c>
-      <c r="B37" s="54"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="55"/>
-      <c r="N37" s="55"/>
-      <c r="O37" s="55"/>
-      <c r="P37" s="55"/>
-      <c r="Q37" s="55"/>
-      <c r="R37" s="55"/>
-      <c r="S37" s="56"/>
-      <c r="T37" s="56"/>
-      <c r="U37" s="56"/>
-      <c r="V37" s="56"/>
-      <c r="W37" s="55"/>
-      <c r="X37" s="55"/>
-      <c r="Y37" s="55"/>
-      <c r="Z37" s="55"/>
-      <c r="AA37" s="55"/>
-      <c r="AB37" s="57"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="59"/>
+      <c r="U37" s="59"/>
+      <c r="V37" s="59"/>
+      <c r="W37" s="58"/>
+      <c r="X37" s="58"/>
+      <c r="Y37" s="58"/>
+      <c r="Z37" s="58"/>
+      <c r="AA37" s="58"/>
+      <c r="AB37" s="60"/>
     </row>
     <row r="38" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="58" t="n">
+      <c r="A38" s="61" t="n">
         <v>14</v>
       </c>
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="60"/>
-      <c r="M38" s="60"/>
-      <c r="N38" s="60"/>
-      <c r="O38" s="60"/>
-      <c r="P38" s="60"/>
-      <c r="Q38" s="60"/>
-      <c r="R38" s="60"/>
-      <c r="S38" s="61"/>
-      <c r="T38" s="61"/>
-      <c r="U38" s="61"/>
-      <c r="V38" s="61"/>
-      <c r="W38" s="60"/>
-      <c r="X38" s="60"/>
-      <c r="Y38" s="60"/>
-      <c r="Z38" s="60"/>
-      <c r="AA38" s="60"/>
-      <c r="AB38" s="62"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
+      <c r="K38" s="63"/>
+      <c r="L38" s="63"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="63"/>
+      <c r="O38" s="63"/>
+      <c r="P38" s="63"/>
+      <c r="Q38" s="63"/>
+      <c r="R38" s="63"/>
+      <c r="S38" s="64"/>
+      <c r="T38" s="64"/>
+      <c r="U38" s="64"/>
+      <c r="V38" s="64"/>
+      <c r="W38" s="63"/>
+      <c r="X38" s="63"/>
+      <c r="Y38" s="63"/>
+      <c r="Z38" s="63"/>
+      <c r="AA38" s="63"/>
+      <c r="AB38" s="65"/>
     </row>
     <row r="39" s="10" customFormat="true" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="66"/>
+      <c r="J39" s="66"/>
+      <c r="K39" s="66"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="66"/>
+      <c r="N39" s="66"/>
+      <c r="O39" s="66"/>
+      <c r="P39" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="63" t="s">
+      <c r="Q39" s="66"/>
+      <c r="R39" s="66"/>
+      <c r="S39" s="66"/>
+      <c r="T39" s="66"/>
+      <c r="U39" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="G39" s="63"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="63"/>
-      <c r="J39" s="63"/>
-      <c r="K39" s="63"/>
-      <c r="L39" s="63"/>
-      <c r="M39" s="63"/>
-      <c r="N39" s="63"/>
-      <c r="O39" s="63"/>
-      <c r="P39" s="63" t="s">
+      <c r="V39" s="66"/>
+      <c r="W39" s="66"/>
+      <c r="X39" s="66"/>
+      <c r="Y39" s="66"/>
+      <c r="Z39" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="Q39" s="63"/>
-      <c r="R39" s="63"/>
-      <c r="S39" s="63"/>
-      <c r="T39" s="63"/>
-      <c r="U39" s="63" t="s">
-        <v>103</v>
-      </c>
-      <c r="V39" s="63"/>
-      <c r="W39" s="63"/>
-      <c r="X39" s="63"/>
-      <c r="Y39" s="63"/>
-      <c r="Z39" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA39" s="64"/>
-      <c r="AB39" s="64"/>
+      <c r="AA39" s="67"/>
+      <c r="AB39" s="67"/>
     </row>
     <row r="40" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="65" t="s">
+      <c r="A40" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
+      <c r="F40" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="69"/>
+      <c r="K40" s="69"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="66" t="s">
+      <c r="Q40" s="69"/>
+      <c r="R40" s="69"/>
+      <c r="S40" s="69"/>
+      <c r="T40" s="69"/>
+      <c r="U40" s="69" t="s">
         <v>106</v>
       </c>
-      <c r="G40" s="66"/>
-      <c r="H40" s="66"/>
-      <c r="I40" s="66"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="66"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="66"/>
-      <c r="N40" s="66"/>
-      <c r="O40" s="66"/>
-      <c r="P40" s="66" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q40" s="66"/>
-      <c r="R40" s="66"/>
-      <c r="S40" s="66"/>
-      <c r="T40" s="66"/>
-      <c r="U40" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="V40" s="66"/>
-      <c r="W40" s="66"/>
-      <c r="X40" s="66"/>
-      <c r="Y40" s="66"/>
-      <c r="Z40" s="67"/>
-      <c r="AA40" s="67"/>
-      <c r="AB40" s="67"/>
+      <c r="V40" s="69"/>
+      <c r="W40" s="69"/>
+      <c r="X40" s="69"/>
+      <c r="Y40" s="69"/>
+      <c r="Z40" s="70"/>
+      <c r="AA40" s="70"/>
+      <c r="AB40" s="70"/>
     </row>
     <row r="41" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="65" t="s">
+      <c r="A41" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="68"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71"/>
+      <c r="L41" s="71"/>
+      <c r="M41" s="71"/>
+      <c r="N41" s="71"/>
+      <c r="O41" s="71"/>
+      <c r="P41" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q41" s="71"/>
+      <c r="R41" s="71"/>
+      <c r="S41" s="71"/>
+      <c r="T41" s="71"/>
+      <c r="U41" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="B41" s="65"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="68"/>
-      <c r="K41" s="68"/>
-      <c r="L41" s="68"/>
-      <c r="M41" s="68"/>
-      <c r="N41" s="68"/>
-      <c r="O41" s="68"/>
-      <c r="P41" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q41" s="68"/>
-      <c r="R41" s="68"/>
-      <c r="S41" s="68"/>
-      <c r="T41" s="68"/>
-      <c r="U41" s="66" t="s">
-        <v>111</v>
-      </c>
-      <c r="V41" s="66"/>
-      <c r="W41" s="66"/>
-      <c r="X41" s="66"/>
-      <c r="Y41" s="66"/>
-      <c r="Z41" s="67"/>
-      <c r="AA41" s="67"/>
-      <c r="AB41" s="67"/>
+      <c r="V41" s="69"/>
+      <c r="W41" s="69"/>
+      <c r="X41" s="69"/>
+      <c r="Y41" s="69"/>
+      <c r="Z41" s="70"/>
+      <c r="AA41" s="70"/>
+      <c r="AB41" s="70"/>
     </row>
     <row r="42" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="65" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="69" t="n">
+      <c r="A42" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="68"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="72" t="n">
         <v>43754</v>
       </c>
-      <c r="G42" s="69"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="69"/>
-      <c r="K42" s="69"/>
-      <c r="L42" s="69"/>
-      <c r="M42" s="69"/>
-      <c r="N42" s="69"/>
-      <c r="O42" s="69"/>
-      <c r="P42" s="69" t="n">
+      <c r="G42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="72"/>
+      <c r="N42" s="72"/>
+      <c r="O42" s="72"/>
+      <c r="P42" s="72" t="n">
         <v>43754</v>
       </c>
-      <c r="Q42" s="69"/>
-      <c r="R42" s="69"/>
-      <c r="S42" s="69"/>
-      <c r="T42" s="69"/>
-      <c r="U42" s="70" t="n">
+      <c r="Q42" s="72"/>
+      <c r="R42" s="72"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="73" t="n">
         <v>43754</v>
       </c>
-      <c r="V42" s="70"/>
-      <c r="W42" s="70"/>
-      <c r="X42" s="70"/>
-      <c r="Y42" s="70"/>
-      <c r="Z42" s="67"/>
-      <c r="AA42" s="67"/>
-      <c r="AB42" s="67"/>
+      <c r="V42" s="73"/>
+      <c r="W42" s="73"/>
+      <c r="X42" s="73"/>
+      <c r="Y42" s="73"/>
+      <c r="Z42" s="70"/>
+      <c r="AA42" s="70"/>
+      <c r="AB42" s="70"/>
     </row>
     <row r="43" customFormat="false" ht="57.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="71" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="71"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="72"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="72"/>
-      <c r="J43" s="72"/>
-      <c r="K43" s="72"/>
-      <c r="L43" s="72"/>
-      <c r="M43" s="72"/>
-      <c r="N43" s="72"/>
-      <c r="O43" s="72"/>
-      <c r="P43" s="72"/>
-      <c r="Q43" s="72"/>
-      <c r="R43" s="72"/>
-      <c r="S43" s="72"/>
-      <c r="T43" s="72"/>
-      <c r="U43" s="72"/>
-      <c r="V43" s="72"/>
-      <c r="W43" s="72"/>
-      <c r="X43" s="72"/>
-      <c r="Y43" s="72"/>
-      <c r="Z43" s="73"/>
-      <c r="AA43" s="73"/>
-      <c r="AB43" s="73"/>
+      <c r="A43" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="74"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="75"/>
+      <c r="J43" s="75"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="75"/>
+      <c r="N43" s="75"/>
+      <c r="O43" s="75"/>
+      <c r="P43" s="75"/>
+      <c r="Q43" s="75"/>
+      <c r="R43" s="75"/>
+      <c r="S43" s="75"/>
+      <c r="T43" s="75"/>
+      <c r="U43" s="75"/>
+      <c r="V43" s="75"/>
+      <c r="W43" s="75"/>
+      <c r="X43" s="75"/>
+      <c r="Y43" s="75"/>
+      <c r="Z43" s="76"/>
+      <c r="AA43" s="76"/>
+      <c r="AB43" s="76"/>
     </row>
     <row r="44" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="74" t="s">
-        <v>114</v>
-      </c>
-      <c r="B44" s="74"/>
-      <c r="C44" s="74"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="74"/>
-      <c r="I44" s="74"/>
-      <c r="J44" s="74"/>
-      <c r="K44" s="74"/>
-      <c r="L44" s="74"/>
-      <c r="M44" s="74"/>
-      <c r="N44" s="74"/>
-      <c r="O44" s="74"/>
-      <c r="P44" s="74"/>
-      <c r="Q44" s="74"/>
-      <c r="R44" s="74"/>
-      <c r="S44" s="74"/>
-      <c r="T44" s="74"/>
-      <c r="U44" s="74"/>
-      <c r="V44" s="74"/>
-      <c r="W44" s="74"/>
-      <c r="X44" s="74"/>
-      <c r="Y44" s="74"/>
-      <c r="Z44" s="74"/>
-      <c r="AA44" s="74"/>
-      <c r="AB44" s="74"/>
+      <c r="A44" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="77"/>
+      <c r="J44" s="77"/>
+      <c r="K44" s="77"/>
+      <c r="L44" s="77"/>
+      <c r="M44" s="77"/>
+      <c r="N44" s="77"/>
+      <c r="O44" s="77"/>
+      <c r="P44" s="77"/>
+      <c r="Q44" s="77"/>
+      <c r="R44" s="77"/>
+      <c r="S44" s="77"/>
+      <c r="T44" s="77"/>
+      <c r="U44" s="77"/>
+      <c r="V44" s="77"/>
+      <c r="W44" s="77"/>
+      <c r="X44" s="77"/>
+      <c r="Y44" s="77"/>
+      <c r="Z44" s="77"/>
+      <c r="AA44" s="77"/>
+      <c r="AB44" s="77"/>
     </row>
     <row r="45" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
improved the tagging of errors withing log
</commit_message>
<xml_diff>
--- a/implicaspection/report-exports/a2yorumkod-Bericht2_MitKommentaren220200601-22:25:22.xlsx
+++ b/implicaspection/report-exports/a2yorumkod-Bericht2_MitKommentaren220200601-22:25:22.xlsx
@@ -3029,7 +3029,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3058,6 +3058,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF21409A"/>
         <bgColor rgb="FF003366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1C1C1C"/>
+        <bgColor rgb="FF333300"/>
       </patternFill>
     </fill>
   </fills>
@@ -3221,7 +3227,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3416,6 +3422,14 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3600,7 +3614,7 @@
       <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF21409A"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF1C1C1C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -3693,7 +3707,7 @@
   <dimension ref="A1:AO74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE20" activeCellId="0" sqref="AE20"/>
+      <selection pane="topLeft" activeCell="AD6" activeCellId="0" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4525,107 +4539,109 @@
       <c r="Z20" s="48"/>
       <c r="AA20" s="48"/>
       <c r="AB20" s="48"/>
+      <c r="AF20" s="49"/>
+      <c r="AG20" s="50"/>
     </row>
     <row r="21" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50" t="n">
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="52" t="n">
         <v>43754</v>
       </c>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="50"/>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="50"/>
-      <c r="S21" s="50"/>
-      <c r="T21" s="50"/>
-      <c r="U21" s="50"/>
-      <c r="V21" s="50"/>
-      <c r="W21" s="50"/>
-      <c r="X21" s="50"/>
-      <c r="Y21" s="50"/>
-      <c r="Z21" s="50"/>
-      <c r="AA21" s="50"/>
-      <c r="AB21" s="50"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="52"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="52"/>
+      <c r="T21" s="52"/>
+      <c r="U21" s="52"/>
+      <c r="V21" s="52"/>
+      <c r="W21" s="52"/>
+      <c r="X21" s="52"/>
+      <c r="Y21" s="52"/>
+      <c r="Z21" s="52"/>
+      <c r="AA21" s="52"/>
+      <c r="AB21" s="52"/>
     </row>
     <row r="22" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="52"/>
-      <c r="P22" s="52"/>
-      <c r="Q22" s="52"/>
-      <c r="R22" s="52"/>
-      <c r="S22" s="52"/>
-      <c r="T22" s="52"/>
-      <c r="U22" s="52"/>
-      <c r="V22" s="52"/>
-      <c r="W22" s="52"/>
-      <c r="X22" s="52"/>
-      <c r="Y22" s="52"/>
-      <c r="Z22" s="52"/>
-      <c r="AA22" s="52"/>
-      <c r="AB22" s="52"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="54"/>
+      <c r="T22" s="54"/>
+      <c r="U22" s="54"/>
+      <c r="V22" s="54"/>
+      <c r="W22" s="54"/>
+      <c r="X22" s="54"/>
+      <c r="Y22" s="54"/>
+      <c r="Z22" s="54"/>
+      <c r="AA22" s="54"/>
+      <c r="AB22" s="54"/>
     </row>
     <row r="23" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="53"/>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="53"/>
-      <c r="S23" s="53"/>
-      <c r="T23" s="53"/>
-      <c r="U23" s="53"/>
-      <c r="V23" s="53"/>
-      <c r="W23" s="53"/>
-      <c r="X23" s="53"/>
-      <c r="Y23" s="53"/>
-      <c r="Z23" s="53"/>
-      <c r="AA23" s="53"/>
-      <c r="AB23" s="53"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="55"/>
+      <c r="T23" s="55"/>
+      <c r="U23" s="55"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="55"/>
+      <c r="Y23" s="55"/>
+      <c r="Z23" s="55"/>
+      <c r="AA23" s="55"/>
+      <c r="AB23" s="55"/>
     </row>
     <row r="24" s="10" customFormat="true" ht="28.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="56" t="s">
         <v>80</v>
       </c>
       <c r="B24" s="27" t="s">
@@ -4668,541 +4684,541 @@
       </c>
       <c r="Z24" s="27"/>
       <c r="AA24" s="27"/>
-      <c r="AB24" s="55" t="s">
+      <c r="AB24" s="57" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="56" t="n">
+      <c r="A25" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="58" t="n">
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="60" t="n">
         <v>300</v>
       </c>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58" t="s">
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58" t="n">
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="60"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="60" t="n">
         <v>12</v>
       </c>
-      <c r="S25" s="59" t="s">
+      <c r="S25" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="T25" s="59"/>
-      <c r="U25" s="59"/>
-      <c r="V25" s="59"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="58"/>
-      <c r="Y25" s="58"/>
-      <c r="Z25" s="58"/>
-      <c r="AA25" s="58"/>
-      <c r="AB25" s="60" t="s">
+      <c r="T25" s="61"/>
+      <c r="U25" s="61"/>
+      <c r="V25" s="61"/>
+      <c r="W25" s="60"/>
+      <c r="X25" s="60"/>
+      <c r="Y25" s="60"/>
+      <c r="Z25" s="60"/>
+      <c r="AA25" s="60"/>
+      <c r="AB25" s="62" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="56" t="n">
+      <c r="A26" s="58" t="n">
         <v>2</v>
       </c>
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="58" t="n">
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="60" t="n">
         <v>300</v>
       </c>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58" t="s">
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="58" t="n">
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="60"/>
+      <c r="Q26" s="60"/>
+      <c r="R26" s="60" t="n">
         <v>12</v>
       </c>
-      <c r="S26" s="59" t="s">
+      <c r="S26" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="T26" s="59"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="59"/>
-      <c r="W26" s="58"/>
-      <c r="X26" s="58"/>
-      <c r="Y26" s="58"/>
-      <c r="Z26" s="58"/>
-      <c r="AA26" s="58"/>
-      <c r="AB26" s="60" t="s">
+      <c r="T26" s="61"/>
+      <c r="U26" s="61"/>
+      <c r="V26" s="61"/>
+      <c r="W26" s="60"/>
+      <c r="X26" s="60"/>
+      <c r="Y26" s="60"/>
+      <c r="Z26" s="60"/>
+      <c r="AA26" s="60"/>
+      <c r="AB26" s="62" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="56" t="n">
+      <c r="A27" s="58" t="n">
         <v>3</v>
       </c>
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="58" t="n">
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="60" t="n">
         <v>300</v>
       </c>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58" t="s">
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58" t="n">
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="60" t="n">
         <v>12</v>
       </c>
-      <c r="S27" s="59" t="s">
+      <c r="S27" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="T27" s="59"/>
-      <c r="U27" s="59"/>
-      <c r="V27" s="59"/>
-      <c r="W27" s="58"/>
-      <c r="X27" s="58"/>
-      <c r="Y27" s="58"/>
-      <c r="Z27" s="58"/>
-      <c r="AA27" s="58"/>
-      <c r="AB27" s="60" t="s">
+      <c r="T27" s="61"/>
+      <c r="U27" s="61"/>
+      <c r="V27" s="61"/>
+      <c r="W27" s="60"/>
+      <c r="X27" s="60"/>
+      <c r="Y27" s="60"/>
+      <c r="Z27" s="60"/>
+      <c r="AA27" s="60"/>
+      <c r="AB27" s="62" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="56" t="n">
+      <c r="A28" s="58" t="n">
         <v>4</v>
       </c>
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="58" t="n">
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="60" t="n">
         <v>300</v>
       </c>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58" t="s">
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="58" t="n">
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="60" t="n">
         <v>12</v>
       </c>
-      <c r="S28" s="59" t="s">
+      <c r="S28" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="T28" s="59"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="59"/>
-      <c r="W28" s="58"/>
-      <c r="X28" s="58"/>
-      <c r="Y28" s="58"/>
-      <c r="Z28" s="58"/>
-      <c r="AA28" s="58"/>
-      <c r="AB28" s="60" t="s">
+      <c r="T28" s="61"/>
+      <c r="U28" s="61"/>
+      <c r="V28" s="61"/>
+      <c r="W28" s="60"/>
+      <c r="X28" s="60"/>
+      <c r="Y28" s="60"/>
+      <c r="Z28" s="60"/>
+      <c r="AA28" s="60"/>
+      <c r="AB28" s="62" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="56" t="n">
+      <c r="A29" s="58" t="n">
         <v>5</v>
       </c>
-      <c r="B29" s="57" t="s">
+      <c r="B29" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="58" t="n">
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="60" t="n">
         <v>300</v>
       </c>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="58" t="s">
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="M29" s="58"/>
-      <c r="N29" s="58"/>
-      <c r="O29" s="58"/>
-      <c r="P29" s="58"/>
-      <c r="Q29" s="58"/>
-      <c r="R29" s="58" t="n">
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="60"/>
+      <c r="R29" s="60" t="n">
         <v>12</v>
       </c>
-      <c r="S29" s="59" t="s">
+      <c r="S29" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="T29" s="59"/>
-      <c r="U29" s="59"/>
-      <c r="V29" s="59"/>
-      <c r="W29" s="58"/>
-      <c r="X29" s="58"/>
-      <c r="Y29" s="58"/>
-      <c r="Z29" s="58"/>
-      <c r="AA29" s="58"/>
-      <c r="AB29" s="60" t="s">
+      <c r="T29" s="61"/>
+      <c r="U29" s="61"/>
+      <c r="V29" s="61"/>
+      <c r="W29" s="60"/>
+      <c r="X29" s="60"/>
+      <c r="Y29" s="60"/>
+      <c r="Z29" s="60"/>
+      <c r="AA29" s="60"/>
+      <c r="AB29" s="62" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="56" t="n">
+      <c r="A30" s="58" t="n">
         <v>6</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="58" t="n">
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="60" t="n">
         <v>300</v>
       </c>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58" t="s">
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58" t="n">
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="60" t="n">
         <v>12</v>
       </c>
-      <c r="S30" s="59" t="s">
+      <c r="S30" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="T30" s="59"/>
-      <c r="U30" s="59"/>
-      <c r="V30" s="59"/>
-      <c r="W30" s="58"/>
-      <c r="X30" s="58"/>
-      <c r="Y30" s="58"/>
-      <c r="Z30" s="58"/>
-      <c r="AA30" s="58"/>
-      <c r="AB30" s="60" t="s">
+      <c r="T30" s="61"/>
+      <c r="U30" s="61"/>
+      <c r="V30" s="61"/>
+      <c r="W30" s="60"/>
+      <c r="X30" s="60"/>
+      <c r="Y30" s="60"/>
+      <c r="Z30" s="60"/>
+      <c r="AA30" s="60"/>
+      <c r="AB30" s="62" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="56" t="n">
+      <c r="A31" s="58" t="n">
         <v>7</v>
       </c>
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="58" t="n">
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60" t="n">
         <v>300</v>
       </c>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58" t="s">
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="58" t="n">
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="60"/>
+      <c r="R31" s="60" t="n">
         <v>4</v>
       </c>
-      <c r="S31" s="59" t="s">
+      <c r="S31" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="T31" s="59"/>
-      <c r="U31" s="59"/>
-      <c r="V31" s="59"/>
-      <c r="W31" s="58"/>
-      <c r="X31" s="58"/>
-      <c r="Y31" s="58"/>
-      <c r="Z31" s="58"/>
-      <c r="AA31" s="58"/>
-      <c r="AB31" s="60" t="s">
+      <c r="T31" s="61"/>
+      <c r="U31" s="61"/>
+      <c r="V31" s="61"/>
+      <c r="W31" s="60"/>
+      <c r="X31" s="60"/>
+      <c r="Y31" s="60"/>
+      <c r="Z31" s="60"/>
+      <c r="AA31" s="60"/>
+      <c r="AB31" s="62" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="56" t="n">
+      <c r="A32" s="58" t="n">
         <v>8</v>
       </c>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="59"/>
-      <c r="T32" s="59"/>
-      <c r="U32" s="59"/>
-      <c r="V32" s="59"/>
-      <c r="W32" s="58"/>
-      <c r="X32" s="58"/>
-      <c r="Y32" s="58"/>
-      <c r="Z32" s="58"/>
-      <c r="AA32" s="58"/>
-      <c r="AB32" s="60"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="60"/>
+      <c r="R32" s="60"/>
+      <c r="S32" s="61"/>
+      <c r="T32" s="61"/>
+      <c r="U32" s="61"/>
+      <c r="V32" s="61"/>
+      <c r="W32" s="60"/>
+      <c r="X32" s="60"/>
+      <c r="Y32" s="60"/>
+      <c r="Z32" s="60"/>
+      <c r="AA32" s="60"/>
+      <c r="AB32" s="62"/>
     </row>
     <row r="33" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="56" t="n">
+      <c r="A33" s="58" t="n">
         <v>9</v>
       </c>
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="58"/>
-      <c r="S33" s="59"/>
-      <c r="T33" s="59"/>
-      <c r="U33" s="59"/>
-      <c r="V33" s="59"/>
-      <c r="W33" s="58"/>
-      <c r="X33" s="58"/>
-      <c r="Y33" s="58"/>
-      <c r="Z33" s="58"/>
-      <c r="AA33" s="58"/>
-      <c r="AB33" s="60"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="61"/>
+      <c r="T33" s="61"/>
+      <c r="U33" s="61"/>
+      <c r="V33" s="61"/>
+      <c r="W33" s="60"/>
+      <c r="X33" s="60"/>
+      <c r="Y33" s="60"/>
+      <c r="Z33" s="60"/>
+      <c r="AA33" s="60"/>
+      <c r="AB33" s="62"/>
     </row>
     <row r="34" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="56" t="n">
+      <c r="A34" s="58" t="n">
         <v>10</v>
       </c>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="59"/>
-      <c r="T34" s="59"/>
-      <c r="U34" s="59"/>
-      <c r="V34" s="59"/>
-      <c r="W34" s="58"/>
-      <c r="X34" s="58"/>
-      <c r="Y34" s="58"/>
-      <c r="Z34" s="58"/>
-      <c r="AA34" s="58"/>
-      <c r="AB34" s="60"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="61"/>
+      <c r="T34" s="61"/>
+      <c r="U34" s="61"/>
+      <c r="V34" s="61"/>
+      <c r="W34" s="60"/>
+      <c r="X34" s="60"/>
+      <c r="Y34" s="60"/>
+      <c r="Z34" s="60"/>
+      <c r="AA34" s="60"/>
+      <c r="AB34" s="62"/>
     </row>
     <row r="35" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="56" t="n">
+      <c r="A35" s="58" t="n">
         <v>11</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="58"/>
-      <c r="S35" s="59"/>
-      <c r="T35" s="59"/>
-      <c r="U35" s="59"/>
-      <c r="V35" s="59"/>
-      <c r="W35" s="58"/>
-      <c r="X35" s="58"/>
-      <c r="Y35" s="58"/>
-      <c r="Z35" s="58"/>
-      <c r="AA35" s="58"/>
-      <c r="AB35" s="60"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="61"/>
+      <c r="T35" s="61"/>
+      <c r="U35" s="61"/>
+      <c r="V35" s="61"/>
+      <c r="W35" s="60"/>
+      <c r="X35" s="60"/>
+      <c r="Y35" s="60"/>
+      <c r="Z35" s="60"/>
+      <c r="AA35" s="60"/>
+      <c r="AB35" s="62"/>
     </row>
     <row r="36" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="56" t="n">
+      <c r="A36" s="58" t="n">
         <v>12</v>
       </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="58"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="58"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="58"/>
-      <c r="R36" s="58"/>
-      <c r="S36" s="59"/>
-      <c r="T36" s="59"/>
-      <c r="U36" s="59"/>
-      <c r="V36" s="59"/>
-      <c r="W36" s="58"/>
-      <c r="X36" s="58"/>
-      <c r="Y36" s="58"/>
-      <c r="Z36" s="58"/>
-      <c r="AA36" s="58"/>
-      <c r="AB36" s="60"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="60"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="61"/>
+      <c r="T36" s="61"/>
+      <c r="U36" s="61"/>
+      <c r="V36" s="61"/>
+      <c r="W36" s="60"/>
+      <c r="X36" s="60"/>
+      <c r="Y36" s="60"/>
+      <c r="Z36" s="60"/>
+      <c r="AA36" s="60"/>
+      <c r="AB36" s="62"/>
     </row>
     <row r="37" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="56" t="n">
+      <c r="A37" s="58" t="n">
         <v>13</v>
       </c>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="58"/>
-      <c r="M37" s="58"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="59"/>
-      <c r="T37" s="59"/>
-      <c r="U37" s="59"/>
-      <c r="V37" s="59"/>
-      <c r="W37" s="58"/>
-      <c r="X37" s="58"/>
-      <c r="Y37" s="58"/>
-      <c r="Z37" s="58"/>
-      <c r="AA37" s="58"/>
-      <c r="AB37" s="60"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="61"/>
+      <c r="T37" s="61"/>
+      <c r="U37" s="61"/>
+      <c r="V37" s="61"/>
+      <c r="W37" s="60"/>
+      <c r="X37" s="60"/>
+      <c r="Y37" s="60"/>
+      <c r="Z37" s="60"/>
+      <c r="AA37" s="60"/>
+      <c r="AB37" s="62"/>
     </row>
     <row r="38" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="61" t="n">
+      <c r="A38" s="63" t="n">
         <v>14</v>
       </c>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
-      <c r="K38" s="63"/>
-      <c r="L38" s="63"/>
-      <c r="M38" s="63"/>
-      <c r="N38" s="63"/>
-      <c r="O38" s="63"/>
-      <c r="P38" s="63"/>
-      <c r="Q38" s="63"/>
-      <c r="R38" s="63"/>
-      <c r="S38" s="64"/>
-      <c r="T38" s="64"/>
-      <c r="U38" s="64"/>
-      <c r="V38" s="64"/>
-      <c r="W38" s="63"/>
-      <c r="X38" s="63"/>
-      <c r="Y38" s="63"/>
-      <c r="Z38" s="63"/>
-      <c r="AA38" s="63"/>
-      <c r="AB38" s="65"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
+      <c r="N38" s="65"/>
+      <c r="O38" s="65"/>
+      <c r="P38" s="65"/>
+      <c r="Q38" s="65"/>
+      <c r="R38" s="65"/>
+      <c r="S38" s="66"/>
+      <c r="T38" s="66"/>
+      <c r="U38" s="66"/>
+      <c r="V38" s="66"/>
+      <c r="W38" s="65"/>
+      <c r="X38" s="65"/>
+      <c r="Y38" s="65"/>
+      <c r="Z38" s="65"/>
+      <c r="AA38" s="65"/>
+      <c r="AB38" s="67"/>
     </row>
     <row r="39" s="10" customFormat="true" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="47" t="s">
@@ -5212,215 +5228,215 @@
       <c r="C39" s="47"/>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
-      <c r="F39" s="66" t="s">
+      <c r="F39" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="G39" s="66"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="66"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="66"/>
-      <c r="L39" s="66"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="66"/>
-      <c r="O39" s="66"/>
-      <c r="P39" s="66" t="s">
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="68"/>
+      <c r="N39" s="68"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="Q39" s="66"/>
-      <c r="R39" s="66"/>
-      <c r="S39" s="66"/>
-      <c r="T39" s="66"/>
-      <c r="U39" s="66" t="s">
+      <c r="Q39" s="68"/>
+      <c r="R39" s="68"/>
+      <c r="S39" s="68"/>
+      <c r="T39" s="68"/>
+      <c r="U39" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="V39" s="66"/>
-      <c r="W39" s="66"/>
-      <c r="X39" s="66"/>
-      <c r="Y39" s="66"/>
-      <c r="Z39" s="67" t="s">
+      <c r="V39" s="68"/>
+      <c r="W39" s="68"/>
+      <c r="X39" s="68"/>
+      <c r="Y39" s="68"/>
+      <c r="Z39" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="AA39" s="67"/>
-      <c r="AB39" s="67"/>
+      <c r="AA39" s="69"/>
+      <c r="AB39" s="69"/>
     </row>
     <row r="40" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="68" t="s">
+      <c r="A40" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="B40" s="68"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="68"/>
-      <c r="F40" s="69" t="s">
+      <c r="B40" s="70"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="G40" s="69"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="69"/>
-      <c r="J40" s="69"/>
-      <c r="K40" s="69"/>
-      <c r="L40" s="69"/>
-      <c r="M40" s="69"/>
-      <c r="N40" s="69"/>
-      <c r="O40" s="69"/>
-      <c r="P40" s="69" t="s">
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="71"/>
+      <c r="J40" s="71"/>
+      <c r="K40" s="71"/>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71"/>
+      <c r="N40" s="71"/>
+      <c r="O40" s="71"/>
+      <c r="P40" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="Q40" s="69"/>
-      <c r="R40" s="69"/>
-      <c r="S40" s="69"/>
-      <c r="T40" s="69"/>
-      <c r="U40" s="69" t="s">
+      <c r="Q40" s="71"/>
+      <c r="R40" s="71"/>
+      <c r="S40" s="71"/>
+      <c r="T40" s="71"/>
+      <c r="U40" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="V40" s="69"/>
-      <c r="W40" s="69"/>
-      <c r="X40" s="69"/>
-      <c r="Y40" s="69"/>
-      <c r="Z40" s="70"/>
-      <c r="AA40" s="70"/>
-      <c r="AB40" s="70"/>
+      <c r="V40" s="71"/>
+      <c r="W40" s="71"/>
+      <c r="X40" s="71"/>
+      <c r="Y40" s="71"/>
+      <c r="Z40" s="72"/>
+      <c r="AA40" s="72"/>
+      <c r="AB40" s="72"/>
     </row>
     <row r="41" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="68" t="s">
+      <c r="A41" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="68"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="71" t="s">
+      <c r="B41" s="70"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G41" s="71"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="71"/>
-      <c r="L41" s="71"/>
-      <c r="M41" s="71"/>
-      <c r="N41" s="71"/>
-      <c r="O41" s="71"/>
-      <c r="P41" s="71" t="s">
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="73"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="73"/>
+      <c r="M41" s="73"/>
+      <c r="N41" s="73"/>
+      <c r="O41" s="73"/>
+      <c r="P41" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="Q41" s="71"/>
-      <c r="R41" s="71"/>
-      <c r="S41" s="71"/>
-      <c r="T41" s="71"/>
-      <c r="U41" s="69" t="s">
+      <c r="Q41" s="73"/>
+      <c r="R41" s="73"/>
+      <c r="S41" s="73"/>
+      <c r="T41" s="73"/>
+      <c r="U41" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="V41" s="69"/>
-      <c r="W41" s="69"/>
-      <c r="X41" s="69"/>
-      <c r="Y41" s="69"/>
-      <c r="Z41" s="70"/>
-      <c r="AA41" s="70"/>
-      <c r="AB41" s="70"/>
+      <c r="V41" s="71"/>
+      <c r="W41" s="71"/>
+      <c r="X41" s="71"/>
+      <c r="Y41" s="71"/>
+      <c r="Z41" s="72"/>
+      <c r="AA41" s="72"/>
+      <c r="AB41" s="72"/>
     </row>
     <row r="42" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="68" t="s">
+      <c r="A42" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="B42" s="68"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="72" t="n">
+      <c r="B42" s="70"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="74" t="n">
         <v>43754</v>
       </c>
-      <c r="G42" s="72"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="72"/>
-      <c r="M42" s="72"/>
-      <c r="N42" s="72"/>
-      <c r="O42" s="72"/>
-      <c r="P42" s="72" t="n">
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="74"/>
+      <c r="L42" s="74"/>
+      <c r="M42" s="74"/>
+      <c r="N42" s="74"/>
+      <c r="O42" s="74"/>
+      <c r="P42" s="74" t="n">
         <v>43754</v>
       </c>
-      <c r="Q42" s="72"/>
-      <c r="R42" s="72"/>
-      <c r="S42" s="72"/>
-      <c r="T42" s="72"/>
-      <c r="U42" s="73" t="n">
+      <c r="Q42" s="74"/>
+      <c r="R42" s="74"/>
+      <c r="S42" s="74"/>
+      <c r="T42" s="74"/>
+      <c r="U42" s="75" t="n">
         <v>43754</v>
       </c>
-      <c r="V42" s="73"/>
-      <c r="W42" s="73"/>
-      <c r="X42" s="73"/>
-      <c r="Y42" s="73"/>
-      <c r="Z42" s="70"/>
-      <c r="AA42" s="70"/>
-      <c r="AB42" s="70"/>
+      <c r="V42" s="75"/>
+      <c r="W42" s="75"/>
+      <c r="X42" s="75"/>
+      <c r="Y42" s="75"/>
+      <c r="Z42" s="72"/>
+      <c r="AA42" s="72"/>
+      <c r="AB42" s="72"/>
     </row>
     <row r="43" customFormat="false" ht="57.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="74" t="s">
+      <c r="A43" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="B43" s="74"/>
-      <c r="C43" s="74"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="75"/>
-      <c r="I43" s="75"/>
-      <c r="J43" s="75"/>
-      <c r="K43" s="75"/>
-      <c r="L43" s="75"/>
-      <c r="M43" s="75"/>
-      <c r="N43" s="75"/>
-      <c r="O43" s="75"/>
-      <c r="P43" s="75"/>
-      <c r="Q43" s="75"/>
-      <c r="R43" s="75"/>
-      <c r="S43" s="75"/>
-      <c r="T43" s="75"/>
-      <c r="U43" s="75"/>
-      <c r="V43" s="75"/>
-      <c r="W43" s="75"/>
-      <c r="X43" s="75"/>
-      <c r="Y43" s="75"/>
-      <c r="Z43" s="76"/>
-      <c r="AA43" s="76"/>
-      <c r="AB43" s="76"/>
+      <c r="B43" s="76"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="77"/>
+      <c r="J43" s="77"/>
+      <c r="K43" s="77"/>
+      <c r="L43" s="77"/>
+      <c r="M43" s="77"/>
+      <c r="N43" s="77"/>
+      <c r="O43" s="77"/>
+      <c r="P43" s="77"/>
+      <c r="Q43" s="77"/>
+      <c r="R43" s="77"/>
+      <c r="S43" s="77"/>
+      <c r="T43" s="77"/>
+      <c r="U43" s="77"/>
+      <c r="V43" s="77"/>
+      <c r="W43" s="77"/>
+      <c r="X43" s="77"/>
+      <c r="Y43" s="77"/>
+      <c r="Z43" s="78"/>
+      <c r="AA43" s="78"/>
+      <c r="AB43" s="78"/>
     </row>
     <row r="44" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="77" t="s">
+      <c r="A44" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="77"/>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
-      <c r="E44" s="77"/>
-      <c r="F44" s="77"/>
-      <c r="G44" s="77"/>
-      <c r="H44" s="77"/>
-      <c r="I44" s="77"/>
-      <c r="J44" s="77"/>
-      <c r="K44" s="77"/>
-      <c r="L44" s="77"/>
-      <c r="M44" s="77"/>
-      <c r="N44" s="77"/>
-      <c r="O44" s="77"/>
-      <c r="P44" s="77"/>
-      <c r="Q44" s="77"/>
-      <c r="R44" s="77"/>
-      <c r="S44" s="77"/>
-      <c r="T44" s="77"/>
-      <c r="U44" s="77"/>
-      <c r="V44" s="77"/>
-      <c r="W44" s="77"/>
-      <c r="X44" s="77"/>
-      <c r="Y44" s="77"/>
-      <c r="Z44" s="77"/>
-      <c r="AA44" s="77"/>
-      <c r="AB44" s="77"/>
+      <c r="B44" s="79"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="79"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="79"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="79"/>
+      <c r="I44" s="79"/>
+      <c r="J44" s="79"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="79"/>
+      <c r="M44" s="79"/>
+      <c r="N44" s="79"/>
+      <c r="O44" s="79"/>
+      <c r="P44" s="79"/>
+      <c r="Q44" s="79"/>
+      <c r="R44" s="79"/>
+      <c r="S44" s="79"/>
+      <c r="T44" s="79"/>
+      <c r="U44" s="79"/>
+      <c r="V44" s="79"/>
+      <c r="W44" s="79"/>
+      <c r="X44" s="79"/>
+      <c r="Y44" s="79"/>
+      <c r="Z44" s="79"/>
+      <c r="AA44" s="79"/>
+      <c r="AB44" s="79"/>
     </row>
     <row r="45" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>